<commit_message>
Add new stuff by batch_git_push
</commit_message>
<xml_diff>
--- a/surveys/datarobot.com/DataRobot 기능리스트-3_4-김태형-2020-03-04.xlsx
+++ b/surveys/datarobot.com/DataRobot 기능리스트-3_4-김태형-2020-03-04.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="88">
   <si>
     <t xml:space="preserve">구분</t>
   </si>
@@ -101,6 +101,20 @@
 ARIMA, Facebook Prophet, AVG Blender, eXtreme Grandient Boosted Trees Regressor, 
 Ridge Regressor with Forecast Distance Modeling</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">- Supervised
+Cox Proportional Hazards (CoxPH), Deep Learning (Neural Networks)
+Distributed Random Forest (DRF), Generalized Linear Model (GLM)
+Gradient Boosting Machine (GBM), Naïve Bayes Classifier
+Stacked Ensembles, Support Vector Machine (SVM)
+XGBoost
+- Unsupervised
+Aggregator, Generalized Low Rank Models (GLRM)
+Isolation Forest, K-Means Clustering,
+Principal Component Analysis (PCA)
+- Miscellaneous
+Word2vec</t>
   </si>
   <si>
     <t xml:space="preserve">Python</t>
@@ -872,7 +886,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -893,8 +907,8 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -903,6 +917,10 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1001,7 +1019,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1009,7 +1027,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="98.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="46.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="60.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="56.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="42.6"/>
@@ -1052,18 +1070,20 @@
       <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="5"/>
+      <c r="D2" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="E2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1072,16 +1092,16 @@
       <c r="C3" s="3"/>
       <c r="D3" s="5"/>
       <c r="E3" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1090,132 +1110,139 @@
       <c r="C4" s="3"/>
       <c r="D4" s="5"/>
       <c r="E4" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="70" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="67.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
+      <c r="D5" s="5"/>
       <c r="E5" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="70" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="67.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
+      <c r="D6" s="5"/>
       <c r="E6" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="53" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
+      <c r="D7" s="5"/>
       <c r="E7" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
+      <c r="D8" s="5"/>
       <c r="E8" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="67.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
+      <c r="D9" s="5"/>
       <c r="E9" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
+      <c r="D10" s="5"/>
       <c r="E10" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="64.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
+      <c r="D11" s="5"/>
       <c r="E11" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1223,22 +1250,22 @@
         <v>4</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="67.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1246,16 +1273,16 @@
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="E13" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1263,27 +1290,29 @@
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="E14" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:A11"/>
     <mergeCell ref="B2:B11"/>
     <mergeCell ref="C2:C11"/>
+    <mergeCell ref="D2:D11"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="B12:B14"/>
     <mergeCell ref="C12:C14"/>
+    <mergeCell ref="D12:D14"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" display="https://www.python.org/"/>
@@ -1357,7 +1386,7 @@
         <v>6</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="34.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1368,14 +1397,14 @@
         <v>7</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" s="5"/>
+        <v>58</v>
+      </c>
+      <c r="D2" s="8"/>
       <c r="E2" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="I2" s="8" t="s">
         <v>59</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1383,13 +1412,13 @@
         <v>4</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>60</v>
+        <v>47</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>61</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I3" s="2"/>
     </row>
@@ -1429,51 +1458,51 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="10"/>
-      <c r="B1" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" s="10" t="s">
+      <c r="A1" s="11"/>
+      <c r="B1" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="E1" s="10" t="s">
+      <c r="D1" s="11" t="s">
         <v>64</v>
       </c>
+      <c r="E1" s="11" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="66" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="n">
+      <c r="A2" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D2" s="11" t="s">
+      <c r="C2" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="D2" s="12" t="s">
         <v>67</v>
       </c>
+      <c r="E2" s="12" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="103.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="n">
+      <c r="A3" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="D3" s="11" t="s">
+      <c r="B3" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="E3" s="10"/>
+      <c r="D3" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" s="11"/>
     </row>
     <row r="5" customFormat="false" ht="66" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -1483,13 +1512,13 @@
         <v>7</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="99" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1497,23 +1526,23 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1546,72 +1575,72 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>